<commit_message>
Practice 1 - Automation of Spreadsheet Calculation
Your task is to automate the calculation of the difference between two fields in an Excel file (Cash In and Cash Out) and input it in the third column. Unfortunately, the file has accumulated a lot of errors over time. A simple workflow will throw System.Exception because the robot will try to perform math calculations with Int32 variables that contain letters.

Create a workflow that takes as input the excel file attached below and adds the difference between Cash In value and Cash Out value for each row on the Difference column. If the calculation of the difference between the two is successful, set the Status to Success, otherwise set it to either Cash In wrong or Cash Out wrong.

Use Try Catch blocks to catch exceptions when trying to convert Cash In and Cash Out values.
</commit_message>
<xml_diff>
--- a/Practice_1_GblExcepHandr_Automation of Spreadsheet Calculation/resources/Practice1.xlsx
+++ b/Practice_1_GblExcepHandr_Automation of Spreadsheet Calculation/resources/Practice1.xlsx
@@ -3,7 +3,7 @@
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEC5579-D8C0-4035-B3C4-E1C5AEB04515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FAD37B-D4D9-415B-83BD-176DF61D4800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -142,7 +142,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="10">
+  <x:cellStyleXfs count="6">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -159,24 +159,13 @@
     <x:xf numFmtId="14" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="9">
+  <x:cellXfs count="10">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <x:xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -523,570 +512,570 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="7.425781" style="4" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="13.855469" style="4" customWidth="1"/>
-    <x:col min="3" max="3" width="11.570312" style="4" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="25.285156" style="4" customWidth="1"/>
+    <x:col min="1" max="1" width="7.425781" style="5" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="13.855469" style="5" customWidth="1"/>
+    <x:col min="3" max="3" width="11.570312" style="5" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="25.285156" style="5" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="5" t="s">
+      <x:c r="A1" s="6" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="5" t="s">
+      <x:c r="B1" s="6" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="5" t="s">
+      <x:c r="C1" s="6" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="5" t="s">
+      <x:c r="D1" s="6" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="5" t="s">
+      <x:c r="E1" s="6" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="6">
+      <x:c r="A2" s="7">
         <x:v>42125</x:v>
       </x:c>
-      <x:c r="B2" s="7" t="n">
+      <x:c r="B2" s="8" t="n">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="C2" s="7" t="n">
+      <x:c r="C2" s="8" t="n">
         <x:v>241</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="6">
+      <x:c r="A3" s="7">
         <x:v>42156</x:v>
       </x:c>
-      <x:c r="B3" s="7" t="n">
+      <x:c r="B3" s="8" t="n">
         <x:v>77</x:v>
       </x:c>
-      <x:c r="C3" s="7" t="n">
+      <x:c r="C3" s="8" t="n">
         <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="6">
+      <x:c r="A4" s="7">
         <x:v>42186</x:v>
       </x:c>
-      <x:c r="B4" s="7" t="n">
+      <x:c r="B4" s="8" t="n">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="C4" s="7" t="n">
+      <x:c r="C4" s="8" t="n">
         <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="6">
+      <x:c r="A5" s="7">
         <x:v>42217</x:v>
       </x:c>
-      <x:c r="B5" s="7" t="s">
+      <x:c r="B5" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="C5" s="7" t="n">
+      <x:c r="C5" s="8" t="n">
         <x:v>130</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="6">
+      <x:c r="A6" s="7">
         <x:v>42248</x:v>
       </x:c>
-      <x:c r="B6" s="7" t="n">
+      <x:c r="B6" s="8" t="n">
         <x:v>144</x:v>
       </x:c>
-      <x:c r="C6" s="7" t="n">
+      <x:c r="C6" s="8" t="n">
         <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="6">
+      <x:c r="A7" s="7">
         <x:v>42278</x:v>
       </x:c>
-      <x:c r="B7" s="7" t="n">
+      <x:c r="B7" s="8" t="n">
         <x:v>160</x:v>
       </x:c>
-      <x:c r="C7" s="7" t="s">
+      <x:c r="C7" s="8" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="6">
+      <x:c r="A8" s="7">
         <x:v>42309</x:v>
       </x:c>
-      <x:c r="B8" s="7" t="s">
+      <x:c r="B8" s="8" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="C8" s="7" t="n">
+      <x:c r="C8" s="8" t="n">
         <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A9" s="6">
+      <x:c r="A9" s="7">
         <x:v>42339</x:v>
       </x:c>
-      <x:c r="B9" s="7" t="n">
+      <x:c r="B9" s="8" t="n">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="C9" s="7" t="n">
+      <x:c r="C9" s="8" t="n">
         <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A10" s="6">
+      <x:c r="A10" s="7">
         <x:v>42370</x:v>
       </x:c>
-      <x:c r="B10" s="7" t="n">
+      <x:c r="B10" s="8" t="n">
         <x:v>134</x:v>
       </x:c>
-      <x:c r="C10" s="7" t="n">
+      <x:c r="C10" s="8" t="n">
         <x:v>169</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="6">
+      <x:c r="A11" s="7">
         <x:v>42401</x:v>
       </x:c>
-      <x:c r="B11" s="7" t="s">
+      <x:c r="B11" s="8" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C11" s="7" t="s">
+      <x:c r="C11" s="8" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A12" s="6">
+      <x:c r="A12" s="7">
         <x:v>42430</x:v>
       </x:c>
-      <x:c r="B12" s="7" t="n">
+      <x:c r="B12" s="8" t="n">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="C12" s="7" t="n">
+      <x:c r="C12" s="8" t="n">
         <x:v>91</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A13" s="6">
+      <x:c r="A13" s="7">
         <x:v>42461</x:v>
       </x:c>
-      <x:c r="B13" s="7" t="s">
+      <x:c r="B13" s="8" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="C13" s="7" t="n">
+      <x:c r="C13" s="8" t="n">
         <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A14" s="6">
+      <x:c r="A14" s="7">
         <x:v>42491</x:v>
       </x:c>
-      <x:c r="B14" s="7" t="n">
+      <x:c r="B14" s="8" t="n">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="C14" s="7" t="n">
+      <x:c r="C14" s="8" t="n">
         <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A15" s="6">
+      <x:c r="A15" s="7">
         <x:v>42522</x:v>
       </x:c>
-      <x:c r="B15" s="7" t="n">
+      <x:c r="B15" s="8" t="n">
         <x:v>154</x:v>
       </x:c>
-      <x:c r="C15" s="7" t="n">
+      <x:c r="C15" s="8" t="n">
         <x:v>123</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A16" s="6">
+      <x:c r="A16" s="7">
         <x:v>42552</x:v>
       </x:c>
-      <x:c r="B16" s="7" t="n">
+      <x:c r="B16" s="8" t="n">
         <x:v>89</x:v>
       </x:c>
-      <x:c r="C16" s="7" t="n">
+      <x:c r="C16" s="8" t="n">
         <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A17" s="6">
+      <x:c r="A17" s="7">
         <x:v>42583</x:v>
       </x:c>
-      <x:c r="B17" s="7" t="n">
+      <x:c r="B17" s="8" t="n">
         <x:v>143</x:v>
       </x:c>
-      <x:c r="C17" s="7" t="n">
+      <x:c r="C17" s="8" t="n">
         <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A18" s="6">
+      <x:c r="A18" s="7">
         <x:v>42614</x:v>
       </x:c>
-      <x:c r="B18" s="7" t="n">
+      <x:c r="B18" s="8" t="n">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="C18" s="7" t="s">
+      <x:c r="C18" s="8" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A19" s="6">
+      <x:c r="A19" s="7">
         <x:v>42644</x:v>
       </x:c>
-      <x:c r="B19" s="7" t="n">
+      <x:c r="B19" s="8" t="n">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="C19" s="7" t="n">
+      <x:c r="C19" s="8" t="n">
         <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A20" s="6">
+      <x:c r="A20" s="7">
         <x:v>42675</x:v>
       </x:c>
-      <x:c r="B20" s="7" t="n">
+      <x:c r="B20" s="8" t="n">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="C20" s="7" t="s">
+      <x:c r="C20" s="8" t="s">
         <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A21" s="6">
+      <x:c r="A21" s="7">
         <x:v>42705</x:v>
       </x:c>
-      <x:c r="B21" s="7" t="n">
+      <x:c r="B21" s="8" t="n">
         <x:v>160</x:v>
       </x:c>
-      <x:c r="C21" s="7" t="n">
+      <x:c r="C21" s="8" t="n">
         <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A22" s="6">
+      <x:c r="A22" s="7">
         <x:v>42736</x:v>
       </x:c>
-      <x:c r="B22" s="7" t="s">
+      <x:c r="B22" s="8" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="C22" s="7" t="n">
+      <x:c r="C22" s="8" t="n">
         <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A23" s="6">
+      <x:c r="A23" s="7">
         <x:v>42767</x:v>
       </x:c>
-      <x:c r="B23" s="7" t="n">
+      <x:c r="B23" s="8" t="n">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="C23" s="7" t="n">
+      <x:c r="C23" s="8" t="n">
         <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A24" s="6">
+      <x:c r="A24" s="7">
         <x:v>42795</x:v>
       </x:c>
-      <x:c r="B24" s="7" t="n">
+      <x:c r="B24" s="8" t="n">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="C24" s="7" t="s">
+      <x:c r="C24" s="8" t="s">
         <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A25" s="6">
+      <x:c r="A25" s="7">
         <x:v>42826</x:v>
       </x:c>
-      <x:c r="B25" s="7" t="n">
+      <x:c r="B25" s="8" t="n">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="C25" s="7" t="n">
+      <x:c r="C25" s="8" t="n">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A26" s="6">
+      <x:c r="A26" s="7">
         <x:v>42856</x:v>
       </x:c>
-      <x:c r="B26" s="7" t="n">
+      <x:c r="B26" s="8" t="n">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="C26" s="7" t="n">
+      <x:c r="C26" s="8" t="n">
         <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A27" s="6">
+      <x:c r="A27" s="7">
         <x:v>42887</x:v>
       </x:c>
-      <x:c r="B27" s="7" t="n">
+      <x:c r="B27" s="8" t="n">
         <x:v>134</x:v>
       </x:c>
-      <x:c r="C27" s="7" t="n">
+      <x:c r="C27" s="8" t="n">
         <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A28" s="6">
+      <x:c r="A28" s="7">
         <x:v>42917</x:v>
       </x:c>
-      <x:c r="B28" s="7" t="n">
+      <x:c r="B28" s="8" t="n">
         <x:v>229</x:v>
       </x:c>
-      <x:c r="C28" s="7" t="n">
+      <x:c r="C28" s="8" t="n">
         <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A29" s="6">
+      <x:c r="A29" s="7">
         <x:v>42948</x:v>
       </x:c>
-      <x:c r="B29" s="7" t="n">
+      <x:c r="B29" s="8" t="n">
         <x:v>73</x:v>
       </x:c>
-      <x:c r="C29" s="7" t="n">
+      <x:c r="C29" s="8" t="n">
         <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A30" s="6">
+      <x:c r="A30" s="7">
         <x:v>42979</x:v>
       </x:c>
-      <x:c r="B30" s="7" t="s">
+      <x:c r="B30" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="C30" s="7" t="n">
+      <x:c r="C30" s="8" t="n">
         <x:v>89</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A31" s="6">
+      <x:c r="A31" s="7">
         <x:v>43009</x:v>
       </x:c>
-      <x:c r="B31" s="7" t="n">
+      <x:c r="B31" s="8" t="n">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="C31" s="7" t="n">
+      <x:c r="C31" s="8" t="n">
         <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A32" s="6">
+      <x:c r="A32" s="7">
         <x:v>43040</x:v>
       </x:c>
-      <x:c r="B32" s="7" t="n">
+      <x:c r="B32" s="8" t="n">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="C32" s="7" t="s">
+      <x:c r="C32" s="8" t="s">
         <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A33" s="6">
+      <x:c r="A33" s="7">
         <x:v>43070</x:v>
       </x:c>
-      <x:c r="B33" s="7" t="n">
+      <x:c r="B33" s="8" t="n">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="C33" s="7" t="n">
+      <x:c r="C33" s="8" t="n">
         <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A34" s="6">
+      <x:c r="A34" s="7">
         <x:v>43101</x:v>
       </x:c>
-      <x:c r="B34" s="7" t="n">
+      <x:c r="B34" s="8" t="n">
         <x:v>148</x:v>
       </x:c>
-      <x:c r="C34" s="7" t="n">
+      <x:c r="C34" s="8" t="n">
         <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A35" s="6">
+      <x:c r="A35" s="7">
         <x:v>43132</x:v>
       </x:c>
-      <x:c r="B35" s="7" t="n">
+      <x:c r="B35" s="8" t="n">
         <x:v>213</x:v>
       </x:c>
-      <x:c r="C35" s="7" t="s">
+      <x:c r="C35" s="8" t="s">
         <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A36" s="6">
+      <x:c r="A36" s="7">
         <x:v>43160</x:v>
       </x:c>
-      <x:c r="B36" s="7" t="s">
+      <x:c r="B36" s="8" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="C36" s="7" t="n">
+      <x:c r="C36" s="8" t="n">
         <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A37" s="6">
+      <x:c r="A37" s="7">
         <x:v>43191</x:v>
       </x:c>
-      <x:c r="B37" s="7" t="n">
+      <x:c r="B37" s="8" t="n">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="C37" s="7" t="s">
+      <x:c r="C37" s="8" t="s">
         <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A38" s="6">
+      <x:c r="A38" s="7">
         <x:v>43221</x:v>
       </x:c>
-      <x:c r="B38" s="7" t="n">
+      <x:c r="B38" s="8" t="n">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="C38" s="7" t="n">
+      <x:c r="C38" s="8" t="n">
         <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A39" s="6">
+      <x:c r="A39" s="7">
         <x:v>43252</x:v>
       </x:c>
-      <x:c r="B39" s="7" t="n">
+      <x:c r="B39" s="8" t="n">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="C39" s="7" t="n">
+      <x:c r="C39" s="8" t="n">
         <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A40" s="6">
+      <x:c r="A40" s="7">
         <x:v>43282</x:v>
       </x:c>
-      <x:c r="B40" s="7" t="n">
+      <x:c r="B40" s="8" t="n">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="C40" s="7" t="n">
+      <x:c r="C40" s="8" t="n">
         <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A41" s="6">
+      <x:c r="A41" s="7">
         <x:v>43313</x:v>
       </x:c>
-      <x:c r="B41" s="7" t="s">
+      <x:c r="B41" s="8" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="C41" s="7" t="n">
+      <x:c r="C41" s="8" t="n">
         <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A42" s="6">
+      <x:c r="A42" s="7">
         <x:v>43344</x:v>
       </x:c>
-      <x:c r="B42" s="7" t="n">
+      <x:c r="B42" s="8" t="n">
         <x:v>130</x:v>
       </x:c>
-      <x:c r="C42" s="7" t="n">
+      <x:c r="C42" s="8" t="n">
         <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A43" s="6">
+      <x:c r="A43" s="7">
         <x:v>43374</x:v>
       </x:c>
-      <x:c r="B43" s="7" t="s">
+      <x:c r="B43" s="8" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="C43" s="7" t="n">
+      <x:c r="C43" s="8" t="n">
         <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A44" s="6">
+      <x:c r="A44" s="7">
         <x:v>43405</x:v>
       </x:c>
-      <x:c r="B44" s="7" t="n">
+      <x:c r="B44" s="8" t="n">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="C44" s="7" t="n">
+      <x:c r="C44" s="8" t="n">
         <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A45" s="6">
+      <x:c r="A45" s="7">
         <x:v>43435</x:v>
       </x:c>
-      <x:c r="B45" s="7" t="n">
+      <x:c r="B45" s="8" t="n">
         <x:v>88</x:v>
       </x:c>
-      <x:c r="C45" s="7" t="n">
+      <x:c r="C45" s="8" t="n">
         <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A46" s="6">
+      <x:c r="A46" s="7">
         <x:v>43466</x:v>
       </x:c>
-      <x:c r="B46" s="7" t="n">
+      <x:c r="B46" s="8" t="n">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="C46" s="7" t="n">
+      <x:c r="C46" s="8" t="n">
         <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A47" s="6">
+      <x:c r="A47" s="7">
         <x:v>43497</x:v>
       </x:c>
-      <x:c r="B47" s="7" t="n">
+      <x:c r="B47" s="8" t="n">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="C47" s="7" t="n">
+      <x:c r="C47" s="8" t="n">
         <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A48" s="6">
+      <x:c r="A48" s="7">
         <x:v>43525</x:v>
       </x:c>
-      <x:c r="B48" s="7" t="n">
+      <x:c r="B48" s="8" t="n">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="C48" s="7" t="n">
+      <x:c r="C48" s="8" t="n">
         <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A49" s="6">
+      <x:c r="A49" s="7">
         <x:v>43556</x:v>
       </x:c>
-      <x:c r="B49" s="7" t="n">
+      <x:c r="B49" s="8" t="n">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="C49" s="7" t="s">
+      <x:c r="C49" s="8" t="s">
         <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A50" s="6">
+      <x:c r="A50" s="7">
         <x:v>43586</x:v>
       </x:c>
-      <x:c r="B50" s="7" t="n">
+      <x:c r="B50" s="8" t="n">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="C50" s="7" t="n">
+      <x:c r="C50" s="8" t="n">
         <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A51" s="6" t="s"/>
+      <x:c r="A51" s="7" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -1102,822 +1091,808 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E49"/>
+  <x:dimension ref="A1:E50"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
     <x:row r="1" spans="1:5">
-      <x:c r="A1" s="8" t="s">
+      <x:c r="A1" s="5" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="4" t="s">
+      <x:c r="B1" s="5" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="4" t="s">
+      <x:c r="C1" s="5" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="4" t="s">
+      <x:c r="D1" s="5" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="4" t="s">
+      <x:c r="E1" s="5" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5">
-      <x:c r="A2" s="8">
+      <x:c r="A2" s="9">
         <x:v>42125</x:v>
       </x:c>
-      <x:c r="B2" s="4" t="n">
+      <x:c r="B2" s="5" t="n">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="C2" s="4" t="n">
+      <x:c r="C2" s="5" t="n">
         <x:v>241</x:v>
       </x:c>
-      <x:c r="D2" s="4" t="n">
+      <x:c r="D2" s="5" t="n">
         <x:v>226</x:v>
       </x:c>
-      <x:c r="E2" s="4" t="s">
+      <x:c r="E2" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5">
-      <x:c r="A3" s="8">
+      <x:c r="A3" s="9">
         <x:v>42156</x:v>
       </x:c>
-      <x:c r="B3" s="4" t="n">
+      <x:c r="B3" s="5" t="n">
         <x:v>77</x:v>
       </x:c>
-      <x:c r="C3" s="4" t="n">
+      <x:c r="C3" s="5" t="n">
         <x:v>90</x:v>
       </x:c>
-      <x:c r="D3" s="4" t="n">
+      <x:c r="D3" s="5" t="n">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="E3" s="4" t="s">
+      <x:c r="E3" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5">
-      <x:c r="A4" s="8">
+      <x:c r="A4" s="9">
         <x:v>42186</x:v>
       </x:c>
-      <x:c r="B4" s="4" t="n">
+      <x:c r="B4" s="5" t="n">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="C4" s="4" t="n">
+      <x:c r="C4" s="5" t="n">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="D4" s="4" t="n">
+      <x:c r="D4" s="5" t="n">
         <x:v>-20</x:v>
       </x:c>
-      <x:c r="E4" s="4" t="s">
+      <x:c r="E4" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
-      <x:c r="A5" s="8">
+      <x:c r="A5" s="9">
         <x:v>42217</x:v>
       </x:c>
-      <x:c r="B5" s="4" t="s">
+      <x:c r="B5" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="C5" s="4" t="n">
+      <x:c r="C5" s="5" t="n">
         <x:v>130</x:v>
       </x:c>
-      <x:c r="D5" s="4" t="s"/>
-      <x:c r="E5" s="4" t="s">
+      <x:c r="E5" s="5" t="s">
         <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
-      <x:c r="A6" s="8">
+      <x:c r="A6" s="9">
         <x:v>42248</x:v>
       </x:c>
-      <x:c r="B6" s="4" t="n">
+      <x:c r="B6" s="5" t="n">
         <x:v>144</x:v>
       </x:c>
-      <x:c r="C6" s="4" t="n">
+      <x:c r="C6" s="5" t="n">
         <x:v>78</x:v>
       </x:c>
-      <x:c r="D6" s="4" t="n">
+      <x:c r="D6" s="5" t="n">
         <x:v>-66</x:v>
       </x:c>
-      <x:c r="E6" s="4" t="s">
+      <x:c r="E6" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
-      <x:c r="A7" s="8">
+      <x:c r="A7" s="9">
         <x:v>42278</x:v>
       </x:c>
-      <x:c r="B7" s="4" t="n">
+      <x:c r="B7" s="5" t="n">
         <x:v>160</x:v>
       </x:c>
-      <x:c r="C7" s="4" t="s">
+      <x:c r="C7" s="5" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="E7" s="4" t="s">
+      <x:c r="E7" s="5" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
-      <x:c r="A8" s="8">
+      <x:c r="A8" s="9">
         <x:v>42309</x:v>
       </x:c>
-      <x:c r="B8" s="4" t="s">
+      <x:c r="B8" s="5" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="C8" s="4" t="n">
+      <x:c r="C8" s="5" t="n">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="D8" s="4" t="s"/>
-      <x:c r="E8" s="4" t="s">
+      <x:c r="E8" s="5" t="s">
         <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
-      <x:c r="A9" s="8">
+      <x:c r="A9" s="9">
         <x:v>42339</x:v>
       </x:c>
-      <x:c r="B9" s="4" t="n">
+      <x:c r="B9" s="5" t="n">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="C9" s="4" t="n">
+      <x:c r="C9" s="5" t="n">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="D9" s="4" t="n">
+      <x:c r="D9" s="5" t="n">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="E9" s="4" t="s">
+      <x:c r="E9" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
-      <x:c r="A10" s="8">
+      <x:c r="A10" s="9">
         <x:v>42370</x:v>
       </x:c>
-      <x:c r="B10" s="4" t="n">
+      <x:c r="B10" s="5" t="n">
         <x:v>134</x:v>
       </x:c>
-      <x:c r="C10" s="4" t="n">
+      <x:c r="C10" s="5" t="n">
         <x:v>169</x:v>
       </x:c>
-      <x:c r="D10" s="4" t="n">
+      <x:c r="D10" s="5" t="n">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="E10" s="4" t="s">
+      <x:c r="E10" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
-      <x:c r="A11" s="8">
+      <x:c r="A11" s="9">
         <x:v>42401</x:v>
       </x:c>
-      <x:c r="B11" s="4" t="s">
+      <x:c r="B11" s="5" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C11" s="4" t="s">
+      <x:c r="C11" s="5" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D11" s="4" t="s"/>
-      <x:c r="E11" s="4" t="s">
+      <x:c r="E11" s="5" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
-      <x:c r="A12" s="8">
+      <x:c r="A12" s="9">
         <x:v>42430</x:v>
       </x:c>
-      <x:c r="B12" s="4" t="n">
+      <x:c r="B12" s="5" t="n">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="C12" s="4" t="n">
+      <x:c r="C12" s="5" t="n">
         <x:v>91</x:v>
       </x:c>
-      <x:c r="D12" s="4" t="n">
+      <x:c r="D12" s="5" t="n">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="E12" s="4" t="s">
+      <x:c r="E12" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
-      <x:c r="A13" s="8">
+      <x:c r="A13" s="9">
         <x:v>42461</x:v>
       </x:c>
-      <x:c r="B13" s="4" t="s">
+      <x:c r="B13" s="5" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="C13" s="4" t="n">
+      <x:c r="C13" s="5" t="n">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D13" s="4" t="s"/>
-      <x:c r="E13" s="4" t="s">
+      <x:c r="E13" s="5" t="s">
         <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
-      <x:c r="A14" s="8">
+      <x:c r="A14" s="9">
         <x:v>42491</x:v>
       </x:c>
-      <x:c r="B14" s="4" t="n">
+      <x:c r="B14" s="5" t="n">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="C14" s="4" t="n">
+      <x:c r="C14" s="5" t="n">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="D14" s="4" t="n">
+      <x:c r="D14" s="5" t="n">
         <x:v>-16</x:v>
       </x:c>
-      <x:c r="E14" s="4" t="s">
+      <x:c r="E14" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5">
-      <x:c r="A15" s="8">
+      <x:c r="A15" s="9">
         <x:v>42522</x:v>
       </x:c>
-      <x:c r="B15" s="4" t="n">
+      <x:c r="B15" s="5" t="n">
         <x:v>154</x:v>
       </x:c>
-      <x:c r="C15" s="4" t="n">
+      <x:c r="C15" s="5" t="n">
         <x:v>123</x:v>
       </x:c>
-      <x:c r="D15" s="4" t="n">
+      <x:c r="D15" s="5" t="n">
         <x:v>-31</x:v>
       </x:c>
-      <x:c r="E15" s="4" t="s">
+      <x:c r="E15" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5">
-      <x:c r="A16" s="8">
+      <x:c r="A16" s="9">
         <x:v>42552</x:v>
       </x:c>
-      <x:c r="B16" s="4" t="n">
+      <x:c r="B16" s="5" t="n">
         <x:v>89</x:v>
       </x:c>
-      <x:c r="C16" s="4" t="n">
+      <x:c r="C16" s="5" t="n">
         <x:v>73</x:v>
       </x:c>
-      <x:c r="D16" s="4" t="n">
+      <x:c r="D16" s="5" t="n">
         <x:v>-16</x:v>
       </x:c>
-      <x:c r="E16" s="4" t="s">
+      <x:c r="E16" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:5">
-      <x:c r="A17" s="8">
+      <x:c r="A17" s="9">
         <x:v>42583</x:v>
       </x:c>
-      <x:c r="B17" s="4" t="n">
+      <x:c r="B17" s="5" t="n">
         <x:v>143</x:v>
       </x:c>
-      <x:c r="C17" s="4" t="n">
+      <x:c r="C17" s="5" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="D17" s="4" t="n">
+      <x:c r="D17" s="5" t="n">
         <x:v>-104</x:v>
       </x:c>
-      <x:c r="E17" s="4" t="s">
+      <x:c r="E17" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5">
-      <x:c r="A18" s="8">
+      <x:c r="A18" s="9">
         <x:v>42614</x:v>
       </x:c>
-      <x:c r="B18" s="4" t="n">
+      <x:c r="B18" s="5" t="n">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="C18" s="4" t="s">
+      <x:c r="C18" s="5" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="D18" s="4" t="s"/>
-      <x:c r="E18" s="4" t="s">
+      <x:c r="E18" s="5" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:5">
-      <x:c r="A19" s="8">
+      <x:c r="A19" s="9">
         <x:v>42644</x:v>
       </x:c>
-      <x:c r="B19" s="4" t="n">
+      <x:c r="B19" s="5" t="n">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="C19" s="4" t="n">
+      <x:c r="C19" s="5" t="n">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="D19" s="4" t="n">
+      <x:c r="D19" s="5" t="n">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="E19" s="4" t="s">
+      <x:c r="E19" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5">
-      <x:c r="A20" s="8">
+      <x:c r="A20" s="9">
         <x:v>42675</x:v>
       </x:c>
-      <x:c r="B20" s="4" t="n">
+      <x:c r="B20" s="5" t="n">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="C20" s="4" t="s">
+      <x:c r="C20" s="5" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D20" s="4" t="s"/>
-      <x:c r="E20" s="4" t="s">
+      <x:c r="E20" s="5" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:5">
-      <x:c r="A21" s="8">
+      <x:c r="A21" s="9">
         <x:v>42705</x:v>
       </x:c>
-      <x:c r="B21" s="4" t="n">
+      <x:c r="B21" s="5" t="n">
         <x:v>160</x:v>
       </x:c>
-      <x:c r="C21" s="4" t="n">
+      <x:c r="C21" s="5" t="n">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="D21" s="4" t="n">
+      <x:c r="D21" s="5" t="n">
         <x:v>-115</x:v>
       </x:c>
-      <x:c r="E21" s="4" t="s">
+      <x:c r="E21" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:5">
-      <x:c r="A22" s="8">
+      <x:c r="A22" s="9">
         <x:v>42736</x:v>
       </x:c>
-      <x:c r="B22" s="4" t="s">
+      <x:c r="B22" s="5" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="C22" s="4" t="n">
+      <x:c r="C22" s="5" t="n">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="D22" s="4" t="s"/>
-      <x:c r="E22" s="4" t="s">
+      <x:c r="E22" s="5" t="s">
         <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:5">
-      <x:c r="A23" s="8">
+      <x:c r="A23" s="9">
         <x:v>42767</x:v>
       </x:c>
-      <x:c r="B23" s="4" t="n">
+      <x:c r="B23" s="5" t="n">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="C23" s="4" t="n">
+      <x:c r="C23" s="5" t="n">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="D23" s="4" t="n">
+      <x:c r="D23" s="5" t="n">
         <x:v>-29</x:v>
       </x:c>
-      <x:c r="E23" s="4" t="s">
+      <x:c r="E23" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5">
-      <x:c r="A24" s="8">
+      <x:c r="A24" s="9">
         <x:v>42795</x:v>
       </x:c>
-      <x:c r="B24" s="4" t="n">
+      <x:c r="B24" s="5" t="n">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="C24" s="4" t="s">
+      <x:c r="C24" s="5" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="D24" s="4" t="s"/>
-      <x:c r="E24" s="4" t="s">
+      <x:c r="E24" s="5" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:5">
-      <x:c r="A25" s="8">
+      <x:c r="A25" s="9">
         <x:v>42826</x:v>
       </x:c>
-      <x:c r="B25" s="4" t="n">
+      <x:c r="B25" s="5" t="n">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="C25" s="4" t="n">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="D25" s="4" t="n">
+      <x:c r="C25" s="5" t="n">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="D25" s="5" t="n">
         <x:v>-14</x:v>
       </x:c>
-      <x:c r="E25" s="4" t="s">
+      <x:c r="E25" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:5">
-      <x:c r="A26" s="8">
+      <x:c r="A26" s="9">
         <x:v>42856</x:v>
       </x:c>
-      <x:c r="B26" s="4" t="n">
+      <x:c r="B26" s="5" t="n">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="C26" s="4" t="n">
+      <x:c r="C26" s="5" t="n">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D26" s="4" t="n">
+      <x:c r="D26" s="5" t="n">
         <x:v>-10</x:v>
       </x:c>
-      <x:c r="E26" s="4" t="s">
+      <x:c r="E26" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:5">
-      <x:c r="A27" s="8">
+      <x:c r="A27" s="9">
         <x:v>42887</x:v>
       </x:c>
-      <x:c r="B27" s="4" t="n">
+      <x:c r="B27" s="5" t="n">
         <x:v>134</x:v>
       </x:c>
-      <x:c r="C27" s="4" t="n">
+      <x:c r="C27" s="5" t="n">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="D27" s="4" t="n">
+      <x:c r="D27" s="5" t="n">
         <x:v>-79</x:v>
       </x:c>
-      <x:c r="E27" s="4" t="s">
+      <x:c r="E27" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:5">
-      <x:c r="A28" s="8">
+      <x:c r="A28" s="9">
         <x:v>42917</x:v>
       </x:c>
-      <x:c r="B28" s="4" t="n">
+      <x:c r="B28" s="5" t="n">
         <x:v>229</x:v>
       </x:c>
-      <x:c r="C28" s="4" t="n">
+      <x:c r="C28" s="5" t="n">
         <x:v>87</x:v>
       </x:c>
-      <x:c r="D28" s="4" t="n">
+      <x:c r="D28" s="5" t="n">
         <x:v>-142</x:v>
       </x:c>
-      <x:c r="E28" s="4" t="s">
+      <x:c r="E28" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:5">
-      <x:c r="A29" s="8">
+      <x:c r="A29" s="9">
         <x:v>42948</x:v>
       </x:c>
-      <x:c r="B29" s="4" t="n">
+      <x:c r="B29" s="5" t="n">
         <x:v>73</x:v>
       </x:c>
-      <x:c r="C29" s="4" t="n">
+      <x:c r="C29" s="5" t="n">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="D29" s="4" t="n">
+      <x:c r="D29" s="5" t="n">
         <x:v>-40</x:v>
       </x:c>
-      <x:c r="E29" s="4" t="s">
+      <x:c r="E29" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:5">
-      <x:c r="A30" s="8">
+      <x:c r="A30" s="9">
         <x:v>42979</x:v>
       </x:c>
-      <x:c r="B30" s="4" t="s">
+      <x:c r="B30" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="C30" s="4" t="n">
+      <x:c r="C30" s="5" t="n">
         <x:v>89</x:v>
       </x:c>
-      <x:c r="D30" s="4" t="s"/>
-      <x:c r="E30" s="4" t="s">
+      <x:c r="E30" s="5" t="s">
         <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:5">
-      <x:c r="A31" s="8">
+      <x:c r="A31" s="9">
         <x:v>43009</x:v>
       </x:c>
-      <x:c r="B31" s="4" t="n">
+      <x:c r="B31" s="5" t="n">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="C31" s="4" t="n">
+      <x:c r="C31" s="5" t="n">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="D31" s="4" t="n">
+      <x:c r="D31" s="5" t="n">
         <x:v>-41</x:v>
       </x:c>
-      <x:c r="E31" s="4" t="s">
+      <x:c r="E31" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:5">
-      <x:c r="A32" s="8">
+      <x:c r="A32" s="9">
         <x:v>43040</x:v>
       </x:c>
-      <x:c r="B32" s="4" t="n">
+      <x:c r="B32" s="5" t="n">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="C32" s="4" t="s">
+      <x:c r="C32" s="5" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="D32" s="4" t="s"/>
-      <x:c r="E32" s="4" t="s">
+      <x:c r="E32" s="5" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:5">
-      <x:c r="A33" s="8">
+      <x:c r="A33" s="9">
         <x:v>43070</x:v>
       </x:c>
-      <x:c r="B33" s="4" t="n">
+      <x:c r="B33" s="5" t="n">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="C33" s="4" t="n">
+      <x:c r="C33" s="5" t="n">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="D33" s="4" t="n">
+      <x:c r="D33" s="5" t="n">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="E33" s="4" t="s">
+      <x:c r="E33" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:5">
-      <x:c r="A34" s="8">
+      <x:c r="A34" s="9">
         <x:v>43101</x:v>
       </x:c>
-      <x:c r="B34" s="4" t="n">
+      <x:c r="B34" s="5" t="n">
         <x:v>148</x:v>
       </x:c>
-      <x:c r="C34" s="4" t="n">
+      <x:c r="C34" s="5" t="n">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="D34" s="4" t="n">
+      <x:c r="D34" s="5" t="n">
         <x:v>-93</x:v>
       </x:c>
-      <x:c r="E34" s="4" t="s">
+      <x:c r="E34" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:5">
-      <x:c r="A35" s="8">
+      <x:c r="A35" s="9">
         <x:v>43132</x:v>
       </x:c>
-      <x:c r="B35" s="4" t="n">
+      <x:c r="B35" s="5" t="n">
         <x:v>213</x:v>
       </x:c>
-      <x:c r="C35" s="4" t="s">
+      <x:c r="C35" s="5" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="E35" s="4" t="s">
+      <x:c r="E35" s="5" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:5">
-      <x:c r="A36" s="8">
+      <x:c r="A36" s="9">
         <x:v>43160</x:v>
       </x:c>
-      <x:c r="B36" s="4" t="s">
+      <x:c r="B36" s="5" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="C36" s="4" t="n">
+      <x:c r="C36" s="5" t="n">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="E36" s="4" t="s">
+      <x:c r="E36" s="5" t="s">
         <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:5">
-      <x:c r="A37" s="8">
+      <x:c r="A37" s="9">
         <x:v>43191</x:v>
       </x:c>
-      <x:c r="B37" s="4" t="n">
+      <x:c r="B37" s="5" t="n">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="C37" s="4" t="s">
+      <x:c r="C37" s="5" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="D37" s="4" t="s"/>
-      <x:c r="E37" s="4" t="s">
+      <x:c r="E37" s="5" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:5">
-      <x:c r="A38" s="8">
+      <x:c r="A38" s="9">
         <x:v>43221</x:v>
       </x:c>
-      <x:c r="B38" s="4" t="n">
+      <x:c r="B38" s="5" t="n">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="C38" s="4" t="n">
+      <x:c r="C38" s="5" t="n">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="D38" s="4" t="n">
+      <x:c r="D38" s="5" t="n">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="E38" s="4" t="s">
+      <x:c r="E38" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:5">
-      <x:c r="A39" s="8">
+      <x:c r="A39" s="9">
         <x:v>43252</x:v>
       </x:c>
-      <x:c r="B39" s="4" t="n">
+      <x:c r="B39" s="5" t="n">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="C39" s="4" t="n">
+      <x:c r="C39" s="5" t="n">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="D39" s="4" t="n">
+      <x:c r="D39" s="5" t="n">
         <x:v>-43</x:v>
       </x:c>
-      <x:c r="E39" s="4" t="s">
+      <x:c r="E39" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:5">
-      <x:c r="A40" s="8">
+      <x:c r="A40" s="9">
         <x:v>43282</x:v>
       </x:c>
-      <x:c r="B40" s="4" t="n">
+      <x:c r="B40" s="5" t="n">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="C40" s="4" t="n">
+      <x:c r="C40" s="5" t="n">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="D40" s="4" t="n">
+      <x:c r="D40" s="5" t="n">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="E40" s="4" t="s">
+      <x:c r="E40" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:5">
-      <x:c r="A41" s="8">
+      <x:c r="A41" s="9">
         <x:v>43313</x:v>
       </x:c>
-      <x:c r="B41" s="4" t="s">
+      <x:c r="B41" s="5" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="C41" s="4" t="n">
+      <x:c r="C41" s="5" t="n">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="D41" s="4" t="s"/>
-      <x:c r="E41" s="4" t="s">
+      <x:c r="E41" s="5" t="s">
         <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:5">
-      <x:c r="A42" s="8">
+      <x:c r="A42" s="9">
         <x:v>43344</x:v>
       </x:c>
-      <x:c r="B42" s="4" t="n">
+      <x:c r="B42" s="5" t="n">
         <x:v>130</x:v>
       </x:c>
-      <x:c r="C42" s="4" t="n">
+      <x:c r="C42" s="5" t="n">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D42" s="4" t="n">
+      <x:c r="D42" s="5" t="n">
         <x:v>-118</x:v>
       </x:c>
-      <x:c r="E42" s="4" t="s">
+      <x:c r="E42" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:5">
-      <x:c r="A43" s="8">
+      <x:c r="A43" s="9">
         <x:v>43374</x:v>
       </x:c>
-      <x:c r="B43" s="4" t="s">
+      <x:c r="B43" s="5" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="C43" s="4" t="n">
+      <x:c r="C43" s="5" t="n">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="D43" s="4" t="s"/>
-      <x:c r="E43" s="4" t="s">
+      <x:c r="E43" s="5" t="s">
         <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:5">
-      <x:c r="A44" s="8">
+      <x:c r="A44" s="9">
         <x:v>43405</x:v>
       </x:c>
-      <x:c r="B44" s="4" t="n">
+      <x:c r="B44" s="5" t="n">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="C44" s="4" t="n">
+      <x:c r="C44" s="5" t="n">
         <x:v>77</x:v>
       </x:c>
-      <x:c r="D44" s="4" t="n">
+      <x:c r="D44" s="5" t="n">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="E44" s="4" t="s">
+      <x:c r="E44" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:5">
-      <x:c r="A45" s="8">
+      <x:c r="A45" s="9">
         <x:v>43435</x:v>
       </x:c>
-      <x:c r="B45" s="4" t="n">
+      <x:c r="B45" s="5" t="n">
         <x:v>88</x:v>
       </x:c>
-      <x:c r="C45" s="4" t="n">
+      <x:c r="C45" s="5" t="n">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="D45" s="4" t="n">
+      <x:c r="D45" s="5" t="n">
         <x:v>-64</x:v>
       </x:c>
-      <x:c r="E45" s="4" t="s">
+      <x:c r="E45" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:5">
-      <x:c r="A46" s="8">
+      <x:c r="A46" s="9">
         <x:v>43466</x:v>
       </x:c>
-      <x:c r="B46" s="4" t="n">
+      <x:c r="B46" s="5" t="n">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="C46" s="4" t="n">
+      <x:c r="C46" s="5" t="n">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D46" s="4" t="n">
+      <x:c r="D46" s="5" t="n">
         <x:v>-2</x:v>
       </x:c>
-      <x:c r="E46" s="4" t="s">
+      <x:c r="E46" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:5">
-      <x:c r="A47" s="8">
+      <x:c r="A47" s="9">
         <x:v>43497</x:v>
       </x:c>
-      <x:c r="B47" s="4" t="n">
+      <x:c r="B47" s="5" t="n">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="C47" s="4" t="n">
+      <x:c r="C47" s="5" t="n">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="D47" s="4" t="n">
+      <x:c r="D47" s="5" t="n">
         <x:v>-26</x:v>
       </x:c>
-      <x:c r="E47" s="4" t="s">
+      <x:c r="E47" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:5">
-      <x:c r="A48" s="8">
+      <x:c r="A48" s="9">
         <x:v>43525</x:v>
       </x:c>
-      <x:c r="B48" s="4" t="n">
+      <x:c r="B48" s="5" t="n">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="C48" s="4" t="n">
+      <x:c r="C48" s="5" t="n">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="D48" s="4" t="n">
+      <x:c r="D48" s="5" t="n">
         <x:v>-36</x:v>
       </x:c>
-      <x:c r="E48" s="4" t="s">
+      <x:c r="E48" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:5">
-      <x:c r="A49" s="8">
+      <x:c r="A49" s="9">
         <x:v>43556</x:v>
       </x:c>
-      <x:c r="B49" s="4" t="n">
+      <x:c r="B49" s="5" t="n">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="C49" s="4" t="s">
+      <x:c r="C49" s="5" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="D49" s="4" t="s"/>
-      <x:c r="E49" s="4" t="s">
+      <x:c r="E49" s="5" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:5">
-      <x:c r="A50" s="8">
+      <x:c r="A50" s="9">
         <x:v>43586</x:v>
       </x:c>
-      <x:c r="B50" s="4" t="n">
+      <x:c r="B50" s="5" t="n">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="C50" s="4" t="n">
+      <x:c r="C50" s="5" t="n">
         <x:v>87</x:v>
       </x:c>
-      <x:c r="D50" s="4" t="n">
+      <x:c r="D50" s="5" t="n">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="E50" s="4" t="s">
+      <x:c r="E50" s="5" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
@@ -1931,12 +1906,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2151,15 +2123,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30C3FB58-143B-4B08-A928-CB6C7DCC9435}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B9BF2ED-C814-4EBF-A991-47D0C74D19DE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2184,10 +2160,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B9BF2ED-C814-4EBF-A991-47D0C74D19DE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30C3FB58-143B-4B08-A928-CB6C7DCC9435}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Practice 1 - Automation of Spreadsheet Calculation - Updated
Handle Exceptions in your client's Cash Flow

Your task is to automate the calculation of the difference between two fields in an Excel file (Cash In and Cash Out) and input it in the third column. Unfortunately, the file has accumulated a lot of errors over time. A simple workflow will throw System.Exception because the robot will try to perform math calculations with Int32 variables that contain letters.

Create a workflow that takes as input the excel file attached below and adds the difference between Cash In value and Cash Out value for each row on the Difference column. If the calculation of the difference between the two is successful, set the Status to Success, otherwise set it to either Cash In wrong or Cash Out wrong.

Use Try Catch blocks to catch exceptions when trying to convert Cash In and Cash Out values.
</commit_message>
<xml_diff>
--- a/Practice_1_GblExcepHandr_Automation of Spreadsheet Calculation/resources/Practice1.xlsx
+++ b/Practice_1_GblExcepHandr_Automation of Spreadsheet Calculation/resources/Practice1.xlsx
@@ -142,7 +142,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="6">
+  <x:cellStyleXfs count="7">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -157,6 +157,9 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="14" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>

</xml_diff>